<commit_message>
Exp 5 done, workin on 6
</commit_message>
<xml_diff>
--- a/Semester8/lab/exp5/exp5data.xlsx
+++ b/Semester8/lab/exp5/exp5data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -351,11 +351,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1130178288"/>
-        <c:axId val="-1130169040"/>
+        <c:axId val="125787536"/>
+        <c:axId val="125782640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1130178288"/>
+        <c:axId val="125787536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -412,12 +412,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1130169040"/>
+        <c:crossAx val="125782640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1130169040"/>
+        <c:axId val="125782640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -474,7 +474,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1130178288"/>
+        <c:crossAx val="125787536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -788,11 +788,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1130165232"/>
-        <c:axId val="-1130182640"/>
+        <c:axId val="125797872"/>
+        <c:axId val="125781552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1130165232"/>
+        <c:axId val="125797872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -849,12 +849,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1130182640"/>
+        <c:crossAx val="125781552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1130182640"/>
+        <c:axId val="125781552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -911,7 +911,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1130165232"/>
+        <c:crossAx val="125797872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2407,7 +2407,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -2682,7 +2682,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>

</xml_diff>